<commit_message>
finish excel table import framework
</commit_message>
<xml_diff>
--- a/Excel Table/TableMap.xlsx
+++ b/Excel Table/TableMap.xlsx
@@ -24,10 +24,10 @@
     <t>scriptObject</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Test</t>
   </si>
   <si>
-    <t>SOTestTable</t>
+    <t>SOTableTest</t>
   </si>
 </sst>
 </file>
@@ -35,10 +35,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -50,12 +50,51 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -63,30 +102,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -100,30 +117,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -172,22 +165,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,19 +202,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,163 +346,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,6 +393,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -414,16 +429,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -444,6 +461,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -458,41 +493,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -501,10 +501,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -513,133 +513,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1000,7 +1000,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
fix issue that table scriptobject is not stable
</commit_message>
<xml_diff>
--- a/Excel Table/TableMap.xlsx
+++ b/Excel Table/TableMap.xlsx
@@ -24,10 +24,10 @@
     <t>scriptObject</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Dialog</t>
   </si>
   <si>
-    <t>SOTableTest</t>
+    <t>SOTableDialog</t>
   </si>
 </sst>
 </file>
@@ -36,9 +36,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -50,6 +50,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -58,15 +65,83 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -81,54 +156,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -140,37 +177,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -179,15 +185,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,43 +202,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +340,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,126 +383,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,17 +396,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -426,46 +440,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,6 +478,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -501,10 +501,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -513,133 +513,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1000,7 +1000,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
scene loading & archive
</commit_message>
<xml_diff>
--- a/Excel Table/TableMap.xlsx
+++ b/Excel Table/TableMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>tableName</t>
   </si>
@@ -29,6 +29,12 @@
   <si>
     <t>SOTableDialog</t>
   </si>
+  <si>
+    <t>UIString</t>
+  </si>
+  <si>
+    <t>SOTableUIString</t>
+  </si>
 </sst>
 </file>
 
@@ -36,9 +42,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -63,9 +69,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -80,22 +161,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,66 +170,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,17 +183,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,79 +208,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,103 +388,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,6 +413,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -416,11 +446,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -436,21 +472,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,21 +499,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -501,10 +507,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -513,133 +519,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -995,15 +1001,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="24.625" customWidth="1"/>
     <col min="2" max="2" width="21.25" customWidth="1"/>
@@ -1023,6 +1029,14 @@
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>